<commit_message>
Added large block with handler of VCM rules
Adjust positions object according to number of VCM crew
</commit_message>
<xml_diff>
--- a/VCM rules.xlsx
+++ b/VCM rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1\CodingJS refactor\crew positions 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1\CodingJS refactor\crew positions 2\crew-positions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>B773 3 class</t>
   </si>
@@ -89,9 +89,6 @@
     <t>L1A move to R2, remove L1A</t>
   </si>
   <si>
-    <t>R1A move to L2, remove R1A</t>
-  </si>
-  <si>
     <t>Keeping Gr2 at LR3 for boarding purposes , R3 must be CSA</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
   </si>
   <si>
     <t>Remove ML1</t>
-  </si>
-  <si>
-    <t>PUR move to ML1, remove PUR</t>
   </si>
   <si>
     <t>UR1A, UL1A must be assigned as per OME
@@ -138,14 +132,91 @@
   <si>
     <t>UR1A, UC1, UL1A must be assigned as per OME
 ML2 and MR4 galleys kept by Gr2, MR3 kept for Gr2 as CSA</t>
+  </si>
+  <si>
+    <t>both ULR and nonULR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PUR move to ML1, ML1 moves to MR1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if CSV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, remove PUR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PUR move to ML1, ML1 moves to MR1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is CSV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, remove PUR</t>
+    </r>
+  </si>
+  <si>
+    <t>R1A move to R2, remove R1A</t>
+  </si>
+  <si>
+    <t>L1A move to L2, remove L1A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -464,15 +535,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -491,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -504,9 +575,6 @@
       <c r="B2">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
@@ -528,7 +596,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -576,9 +644,6 @@
       <c r="B8">
         <v>14</v>
       </c>
-      <c r="C8">
-        <v>11</v>
-      </c>
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -603,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -629,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -642,9 +707,6 @@
       <c r="B13">
         <v>13</v>
       </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
       <c r="D13" t="s">
         <v>2</v>
       </c>
@@ -658,24 +720,24 @@
         <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -684,12 +746,12 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>22</v>
@@ -701,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -714,9 +776,6 @@
       <c r="B19">
         <v>23</v>
       </c>
-      <c r="C19">
-        <v>19</v>
-      </c>
       <c r="D19" t="s">
         <v>2</v>
       </c>
@@ -726,46 +785,49 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
       <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
         <v>26</v>
       </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
         <v>28</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
         <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>21</v>
@@ -777,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>9</v>
@@ -790,9 +852,6 @@
       <c r="B25">
         <v>22</v>
       </c>
-      <c r="C25">
-        <v>20</v>
-      </c>
       <c r="D25" t="s">
         <v>2</v>
       </c>
@@ -802,22 +861,25 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
       <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
         <v>30</v>
       </c>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -835,5 +897,6 @@
     <mergeCell ref="F14:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved visuals of VCMrules
</commit_message>
<xml_diff>
--- a/VCM rules.xlsx
+++ b/VCM rules.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>B773 3 class</t>
   </si>
@@ -200,6 +200,27 @@
   <si>
     <t>L1A move to L2, remove L1A</t>
   </si>
+  <si>
+    <t>Aircraft type</t>
+  </si>
+  <si>
+    <t>Normal crew compliment</t>
+  </si>
+  <si>
+    <t>Minimum crew compliment</t>
+  </si>
+  <si>
+    <t>Number of VCM</t>
+  </si>
+  <si>
+    <t>Main VCM step</t>
+  </si>
+  <si>
+    <t>Additional VCM actions</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
 </sst>
 </file>
 
@@ -225,15 +246,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -241,18 +268,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -533,368 +702,480 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2" s="2">
         <v>14</v>
       </c>
-      <c r="C1">
+      <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="4">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="2">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="2">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G8" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="4">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="2">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G13" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="4">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F18" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="2">
         <v>22</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="2">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G19" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="4">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G21" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="4">
         <v>21</v>
       </c>
-      <c r="C24">
+      <c r="C25" s="4">
         <v>19</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" s="4"/>
+      <c r="E25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G25" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B25">
+      <c r="B26" s="4">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G27" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="G28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>